<commit_message>
added example for auto
</commit_message>
<xml_diff>
--- a/research/matmul-master/results.xlsx
+++ b/research/matmul-master/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chinmaygarg/Box Sync/cs263-project/research/matmul-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F3B4D8-45CC-944A-8036-B868D879D3EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9F23E0-A2FD-284E-A76E-514A2A8E0672}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="16640" activeTab="1" xr2:uid="{74F325F0-6243-AA4C-8826-5AD7F9DE1D95}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>O</t>
   </si>
@@ -78,18 +78,6 @@
   </si>
   <si>
     <t>no vectorization</t>
-  </si>
-  <si>
-    <t>clang</t>
-  </si>
-  <si>
-    <t>g++-8.3</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>not done</t>
   </si>
   <si>
     <t> 0.441047</t>
@@ -4078,10 +4066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9A6CB2-F3B5-284A-A734-3BA97B4296CC}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4095,7 +4083,7 @@
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -4108,7 +4096,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
@@ -4128,7 +4116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4151,7 +4139,7 @@
         <v>1.4129400000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4173,14 +4161,8 @@
       <c r="G4" s="1">
         <v>0.17288799999999999</v>
       </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4202,14 +4184,8 @@
       <c r="G5" s="1">
         <v>0.17338799999999999</v>
       </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -4232,7 +4208,7 @@
         <v>0.17269300000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4266,10 +4242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32609B8-EA14-DC42-8095-D0C36BC6C2A6}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K5" sqref="J4:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4283,7 +4259,7 @@
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -4296,7 +4272,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
@@ -4316,7 +4292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4339,7 +4315,7 @@
         <v>1.7073100000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4361,14 +4337,8 @@
       <c r="G4" s="1">
         <v>0.41569099999999998</v>
       </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4390,14 +4360,8 @@
       <c r="G5" s="1">
         <v>0.407414</v>
       </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -4420,7 +4384,7 @@
         <v>0.40347100000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4428,7 +4392,7 @@
         <v>8.0442999999999998</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1">
         <v>0.413802</v>

</xml_diff>